<commit_message>
include real time tax
</commit_message>
<xml_diff>
--- a/Aluguel/stream-dash/devol.xlsx
+++ b/Aluguel/stream-dash/devol.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="147">
   <si>
     <t>Data</t>
   </si>
@@ -58,9 +58,18 @@
     <t>UBS BRASIL CCTVM S/A</t>
   </si>
   <si>
+    <t>ATIVA INVESTIMENTOS S/A CTCV</t>
+  </si>
+  <si>
     <t>MIRAE ASSET WEALTH MANAGEMENT (BRASIL) CCTVM LTDA.</t>
   </si>
   <si>
+    <t>INTL FCSTONE DTVM LTDA</t>
+  </si>
+  <si>
+    <t>CREDIT SUISSE (BRASIL) S.A. CTVM</t>
+  </si>
+  <si>
     <t>D</t>
   </si>
   <si>
@@ -70,12 +79,51 @@
     <t>ABEV3</t>
   </si>
   <si>
+    <t>B3SA3</t>
+  </si>
+  <si>
+    <t>BBAS3</t>
+  </si>
+  <si>
     <t>BBDC4</t>
   </si>
   <si>
+    <t>BEEF3</t>
+  </si>
+  <si>
+    <t>BPAC11</t>
+  </si>
+  <si>
+    <t>BRAP4</t>
+  </si>
+  <si>
+    <t>BRFS3</t>
+  </si>
+  <si>
+    <t>BRKM5</t>
+  </si>
+  <si>
+    <t>BRML3</t>
+  </si>
+  <si>
+    <t>CCRO3</t>
+  </si>
+  <si>
+    <t>CIEL3</t>
+  </si>
+  <si>
     <t>CMIG4</t>
   </si>
   <si>
+    <t>CMIN3</t>
+  </si>
+  <si>
+    <t>COGN3</t>
+  </si>
+  <si>
+    <t>CPLE6</t>
+  </si>
+  <si>
     <t>CSAN3</t>
   </si>
   <si>
@@ -85,66 +133,174 @@
     <t>CVCB3</t>
   </si>
   <si>
+    <t>DXCO3</t>
+  </si>
+  <si>
     <t>EGIE3</t>
   </si>
   <si>
-    <t>EMBR3</t>
+    <t>ELET6</t>
+  </si>
+  <si>
+    <t>ENBR3</t>
   </si>
   <si>
     <t>EQTL3</t>
   </si>
   <si>
+    <t>EZTC3</t>
+  </si>
+  <si>
+    <t>GGBR4</t>
+  </si>
+  <si>
     <t>GOLL4</t>
   </si>
   <si>
-    <t>JBSS3</t>
+    <t>HYPE3</t>
+  </si>
+  <si>
+    <t>ITUB4</t>
+  </si>
+  <si>
+    <t>JHSF3</t>
+  </si>
+  <si>
+    <t>LCAM3</t>
   </si>
   <si>
     <t>LREN3</t>
   </si>
   <si>
-    <t>LWSA3</t>
-  </si>
-  <si>
     <t>MGLU3</t>
   </si>
   <si>
     <t>MRFG3</t>
   </si>
   <si>
+    <t>MRVE3</t>
+  </si>
+  <si>
     <t>MULT3</t>
   </si>
   <si>
-    <t>PETZ3</t>
-  </si>
-  <si>
-    <t>QUAL3</t>
+    <t>NTCO3</t>
+  </si>
+  <si>
+    <t>PETR3</t>
+  </si>
+  <si>
+    <t>PETR4</t>
+  </si>
+  <si>
+    <t>POSI3</t>
+  </si>
+  <si>
+    <t>RADL3</t>
+  </si>
+  <si>
+    <t>RAIL3</t>
+  </si>
+  <si>
+    <t>RENT3</t>
+  </si>
+  <si>
+    <t>SBSP3</t>
+  </si>
+  <si>
+    <t>SOMA3</t>
   </si>
   <si>
     <t>SUZB3</t>
   </si>
   <si>
+    <t>UGPA3</t>
+  </si>
+  <si>
     <t>VBBR3</t>
   </si>
   <si>
-    <t>WEGE3</t>
+    <t>YDUQ3</t>
   </si>
   <si>
     <t>2022032900339479130001-1</t>
   </si>
   <si>
+    <t>2022033000339702490001-1</t>
+  </si>
+  <si>
+    <t>2022033000339702540001-1</t>
+  </si>
+  <si>
+    <t>2022040600341190420001-1</t>
+  </si>
+  <si>
     <t>2022032900339479240001-1</t>
   </si>
   <si>
     <t>2022033000339702750001-1</t>
   </si>
   <si>
+    <t>2022032400338664970001-1</t>
+  </si>
+  <si>
+    <t>2022040600341190640001-1</t>
+  </si>
+  <si>
+    <t>2022032900339479030001-1</t>
+  </si>
+  <si>
+    <t>2022040600341190440001-1</t>
+  </si>
+  <si>
+    <t>2022032900339479160001-1</t>
+  </si>
+  <si>
+    <t>2022033000339702830001-1</t>
+  </si>
+  <si>
+    <t>2022033100339937010001-1</t>
+  </si>
+  <si>
+    <t>2022032400338664830001-1</t>
+  </si>
+  <si>
+    <t>2022040600341190410001-1</t>
+  </si>
+  <si>
+    <t>2022032900339479230001-1</t>
+  </si>
+  <si>
+    <t>2022033100339936880001-1</t>
+  </si>
+  <si>
+    <t>2022033100339937040001-1</t>
+  </si>
+  <si>
+    <t>2022033100339936910001-1</t>
+  </si>
+  <si>
     <t>2022033000339702720001-1</t>
   </si>
   <si>
+    <t>2022040600341190570001-1</t>
+  </si>
+  <si>
+    <t>2022033000339702740001-1</t>
+  </si>
+  <si>
+    <t>2022032900339479270001-1</t>
+  </si>
+  <si>
+    <t>2022040600341190470001-1</t>
+  </si>
+  <si>
     <t>2022033000339702510001-1</t>
   </si>
   <si>
+    <t>2022032400338664910001-1</t>
+  </si>
+  <si>
     <t>2022033000339702630001-1</t>
   </si>
   <si>
@@ -154,27 +310,57 @@
     <t>2022032400338664780001-1</t>
   </si>
   <si>
+    <t>2022040600341190370001-1</t>
+  </si>
+  <si>
     <t>2022033000339702800001-1</t>
   </si>
   <si>
-    <t>2022033000339702760001-1</t>
+    <t>2022040600341190430001-1</t>
+  </si>
+  <si>
+    <t>2022032400338665030001-1</t>
+  </si>
+  <si>
+    <t>2022040600341190620001-1</t>
   </si>
   <si>
     <t>2022032400338665400001-1</t>
   </si>
   <si>
+    <t>2022040600341190460001-1</t>
+  </si>
+  <si>
+    <t>2022033100339936900001-1</t>
+  </si>
+  <si>
     <t>2022033000339702710001-1</t>
   </si>
   <si>
-    <t>2022033000339702890001-1</t>
+    <t>2022040600341190400001-1</t>
+  </si>
+  <si>
+    <t>2022033100339936990001-1</t>
+  </si>
+  <si>
+    <t>2022040100340215220001-1</t>
+  </si>
+  <si>
+    <t>2022040600341190610001-1</t>
+  </si>
+  <si>
+    <t>2022040600341190600001-1</t>
+  </si>
+  <si>
+    <t>2022033100339937180001-1</t>
+  </si>
+  <si>
+    <t>2022033100339936960001-1</t>
   </si>
   <si>
     <t>2022032400338665050001-1</t>
   </si>
   <si>
-    <t>2022033000339702950001-1</t>
-  </si>
-  <si>
     <t>2022031800337296540001-1</t>
   </si>
   <si>
@@ -184,19 +370,67 @@
     <t>2022032500339018250001-1</t>
   </si>
   <si>
+    <t>2022033100340032460001-1</t>
+  </si>
+  <si>
     <t>2022033000339702990001-1</t>
   </si>
   <si>
+    <t>2022040600341190560001-1</t>
+  </si>
+  <si>
     <t>2022032900339479000001-1</t>
   </si>
   <si>
     <t>2022033000339702770001-1</t>
   </si>
   <si>
-    <t>2022033100339937090001-1</t>
-  </si>
-  <si>
-    <t>2022033000339702900001-1</t>
+    <t>2022040600341190660001-1</t>
+  </si>
+  <si>
+    <t>2022040500340907900001-1</t>
+  </si>
+  <si>
+    <t>2022040500340933200001-1</t>
+  </si>
+  <si>
+    <t>2022040500340933210001-1</t>
+  </si>
+  <si>
+    <t>2022040600341190450001-1</t>
+  </si>
+  <si>
+    <t>2022040500340907960001-1</t>
+  </si>
+  <si>
+    <t>2022040600341190490001-1</t>
+  </si>
+  <si>
+    <t>2022040600341190590001-1</t>
+  </si>
+  <si>
+    <t>2022040600341190550001-1</t>
+  </si>
+  <si>
+    <t>2022033000339702650001-1</t>
+  </si>
+  <si>
+    <t>2022040500340907940001-1</t>
+  </si>
+  <si>
+    <t>2022040600341190630001-1</t>
+  </si>
+  <si>
+    <t>2022033000339702620001-1</t>
+  </si>
+  <si>
+    <t>2022040600341190500001-1</t>
+  </si>
+  <si>
+    <t>2022040500340907970001-1</t>
+  </si>
+  <si>
+    <t>2022040600341190580001-1</t>
   </si>
   <si>
     <t>2022032900339479070001-1</t>
@@ -205,13 +439,22 @@
     <t>2022033000339702980001-1</t>
   </si>
   <si>
+    <t>2022040500340908000001-1</t>
+  </si>
+  <si>
+    <t>2022033100339937160001-1</t>
+  </si>
+  <si>
+    <t>2022040600341190510001-1</t>
+  </si>
+  <si>
     <t>2022033000339702970001-1</t>
   </si>
   <si>
     <t>2022032400338665200001-1</t>
   </si>
   <si>
-    <t>2022033000339702610001-1</t>
+    <t>2022033000339702660001-1</t>
   </si>
 </sst>
 </file>
@@ -573,7 +816,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M29"/>
+  <dimension ref="A1:M79"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -631,7 +874,7 @@
         <v>13</v>
       </c>
       <c r="E2" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F2" s="2">
         <v>44691</v>
@@ -643,27 +886,27 @@
         <v>14.59</v>
       </c>
       <c r="I2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J2" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="K2" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="L2">
         <v>-7247</v>
       </c>
       <c r="M2">
-        <v>-2300</v>
+        <v>-7247</v>
       </c>
     </row>
     <row r="3" spans="1:13">
       <c r="A3" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" s="2">
-        <v>44649</v>
+        <v>44650</v>
       </c>
       <c r="C3" t="s">
         <v>12</v>
@@ -672,36 +915,36 @@
         <v>13</v>
       </c>
       <c r="E3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F3" s="2">
-        <v>44691</v>
+        <v>44692</v>
       </c>
       <c r="G3">
-        <v>0.005</v>
+        <v>0.0021</v>
       </c>
       <c r="H3">
-        <v>22.12</v>
+        <v>15.16</v>
       </c>
       <c r="I3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="K3" t="s">
-        <v>39</v>
+        <v>70</v>
       </c>
       <c r="L3">
-        <v>-2006</v>
+        <v>-40400</v>
       </c>
       <c r="M3">
-        <v>-2006</v>
+        <v>-15853</v>
       </c>
     </row>
     <row r="4" spans="1:13">
       <c r="A4" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" s="2">
         <v>44650</v>
@@ -713,39 +956,39 @@
         <v>13</v>
       </c>
       <c r="E4" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F4" s="2">
         <v>44692</v>
       </c>
       <c r="G4">
-        <v>0.0049</v>
+        <v>0.0003</v>
       </c>
       <c r="H4">
-        <v>22.56</v>
+        <v>15.58</v>
       </c>
       <c r="I4" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J4" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="K4" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="L4">
-        <v>-93253</v>
+        <v>-10800</v>
       </c>
       <c r="M4">
-        <v>-494</v>
+        <v>-3526</v>
       </c>
     </row>
     <row r="5" spans="1:13">
       <c r="A5" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" s="2">
-        <v>44650</v>
+        <v>44657</v>
       </c>
       <c r="C5" t="s">
         <v>12</v>
@@ -754,39 +997,39 @@
         <v>13</v>
       </c>
       <c r="E5" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F5" s="2">
-        <v>44692</v>
+        <v>44699</v>
       </c>
       <c r="G5">
-        <v>0.0016</v>
+        <v>0.0013</v>
       </c>
       <c r="H5">
-        <v>14.7</v>
+        <v>33.6</v>
       </c>
       <c r="I5" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J5" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="K5" t="s">
-        <v>41</v>
+        <v>72</v>
       </c>
       <c r="L5">
-        <v>-12195</v>
+        <v>-13053</v>
       </c>
       <c r="M5">
-        <v>-600</v>
+        <v>-6474</v>
       </c>
     </row>
     <row r="6" spans="1:13">
       <c r="A6" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" s="2">
-        <v>44650</v>
+        <v>44649</v>
       </c>
       <c r="C6" t="s">
         <v>12</v>
@@ -795,36 +1038,36 @@
         <v>13</v>
       </c>
       <c r="E6" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F6" s="2">
-        <v>44692</v>
+        <v>44691</v>
       </c>
       <c r="G6">
-        <v>0.0016</v>
+        <v>0.005</v>
       </c>
       <c r="H6">
-        <v>24.42</v>
+        <v>22.12</v>
       </c>
       <c r="I6" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J6" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="K6" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="L6">
-        <v>-3892</v>
+        <v>-2006</v>
       </c>
       <c r="M6">
-        <v>-600</v>
+        <v>-2006</v>
       </c>
     </row>
     <row r="7" spans="1:13">
       <c r="A7" s="1">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>44650</v>
@@ -836,39 +1079,39 @@
         <v>13</v>
       </c>
       <c r="E7" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F7" s="2">
         <v>44692</v>
       </c>
       <c r="G7">
-        <v>0.0002</v>
+        <v>0.0049</v>
       </c>
       <c r="H7">
-        <v>26.03</v>
+        <v>22.56</v>
       </c>
       <c r="I7" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J7" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="K7" t="s">
-        <v>43</v>
+        <v>74</v>
       </c>
       <c r="L7">
-        <v>-6000</v>
+        <v>-93253</v>
       </c>
       <c r="M7">
-        <v>-6000</v>
+        <v>-22894</v>
       </c>
     </row>
     <row r="8" spans="1:13">
       <c r="A8" s="1">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" s="2">
-        <v>44649</v>
+        <v>44644</v>
       </c>
       <c r="C8" t="s">
         <v>12</v>
@@ -877,39 +1120,39 @@
         <v>13</v>
       </c>
       <c r="E8" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F8" s="2">
-        <v>44691</v>
+        <v>44686</v>
       </c>
       <c r="G8">
-        <v>0.0635</v>
+        <v>0.0044</v>
       </c>
       <c r="H8">
-        <v>15.87</v>
+        <v>11.31</v>
       </c>
       <c r="I8" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J8" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="K8" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="L8">
-        <v>-1515</v>
+        <v>-1892</v>
       </c>
       <c r="M8">
-        <v>-1515</v>
+        <v>-373</v>
       </c>
     </row>
     <row r="9" spans="1:13">
       <c r="A9" s="1">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
-        <v>44644</v>
+        <v>44657</v>
       </c>
       <c r="C9" t="s">
         <v>12</v>
@@ -918,39 +1161,39 @@
         <v>13</v>
       </c>
       <c r="E9" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F9" s="2">
-        <v>44686</v>
+        <v>44699</v>
       </c>
       <c r="G9">
-        <v>0.06809999999999999</v>
+        <v>0.0045</v>
       </c>
       <c r="H9">
-        <v>14.31</v>
+        <v>25.55</v>
       </c>
       <c r="I9" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J9" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="K9" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="L9">
-        <v>-23200</v>
+        <v>-7300</v>
       </c>
       <c r="M9">
-        <v>-20785</v>
+        <v>-1006</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="A10" s="1">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="2">
-        <v>44650</v>
+        <v>44649</v>
       </c>
       <c r="C10" t="s">
         <v>12</v>
@@ -959,39 +1202,39 @@
         <v>13</v>
       </c>
       <c r="E10" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F10" s="2">
-        <v>44692</v>
+        <v>44691</v>
       </c>
       <c r="G10">
-        <v>0.0089</v>
+        <v>0.0057</v>
       </c>
       <c r="H10">
-        <v>43.37</v>
+        <v>33.47</v>
       </c>
       <c r="I10" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J10" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="K10" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="L10">
-        <v>-2400</v>
+        <v>-307</v>
       </c>
       <c r="M10">
-        <v>-200</v>
+        <v>-307</v>
       </c>
     </row>
     <row r="11" spans="1:13">
       <c r="A11" s="1">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11" s="2">
-        <v>44650</v>
+        <v>44657</v>
       </c>
       <c r="C11" t="s">
         <v>12</v>
@@ -1000,39 +1243,39 @@
         <v>13</v>
       </c>
       <c r="E11" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F11" s="2">
-        <v>44692</v>
+        <v>44699</v>
       </c>
       <c r="G11">
-        <v>0.008699999999999999</v>
+        <v>0.0037</v>
       </c>
       <c r="H11">
-        <v>15.69</v>
+        <v>33.89</v>
       </c>
       <c r="I11" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J11" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K11" t="s">
-        <v>47</v>
+        <v>78</v>
       </c>
       <c r="L11">
-        <v>-506</v>
+        <v>-1980</v>
       </c>
       <c r="M11">
-        <v>-400</v>
+        <v>-419</v>
       </c>
     </row>
     <row r="12" spans="1:13">
       <c r="A12" s="1">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B12" s="2">
-        <v>44644</v>
+        <v>44649</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -1041,36 +1284,36 @@
         <v>13</v>
       </c>
       <c r="E12" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F12" s="2">
-        <v>44686</v>
+        <v>44691</v>
       </c>
       <c r="G12">
-        <v>0.003</v>
+        <v>0.0162</v>
       </c>
       <c r="H12">
-        <v>27.06</v>
+        <v>17.4</v>
       </c>
       <c r="I12" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J12" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="K12" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="L12">
-        <v>-8703</v>
+        <v>-3100</v>
       </c>
       <c r="M12">
-        <v>-600</v>
+        <v>-3100</v>
       </c>
     </row>
     <row r="13" spans="1:13">
       <c r="A13" s="1">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B13" s="2">
         <v>44650</v>
@@ -1082,39 +1325,39 @@
         <v>13</v>
       </c>
       <c r="E13" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F13" s="2">
         <v>44692</v>
       </c>
       <c r="G13">
-        <v>0.1866</v>
+        <v>0.0144</v>
       </c>
       <c r="H13">
-        <v>17.73</v>
+        <v>18.06</v>
       </c>
       <c r="I13" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J13" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="K13" t="s">
-        <v>49</v>
+        <v>80</v>
       </c>
       <c r="L13">
-        <v>-1600</v>
+        <v>-10100</v>
       </c>
       <c r="M13">
-        <v>-100</v>
+        <v>-867</v>
       </c>
     </row>
     <row r="14" spans="1:13">
       <c r="A14" s="1">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2">
-        <v>44650</v>
+        <v>44651</v>
       </c>
       <c r="C14" t="s">
         <v>12</v>
@@ -1123,36 +1366,36 @@
         <v>13</v>
       </c>
       <c r="E14" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F14" s="2">
-        <v>44692</v>
+        <v>44693</v>
       </c>
       <c r="G14">
-        <v>0.0007</v>
+        <v>0.0713</v>
       </c>
       <c r="H14">
-        <v>36.29</v>
+        <v>45.65</v>
       </c>
       <c r="I14" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J14" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="K14" t="s">
-        <v>50</v>
+        <v>81</v>
       </c>
       <c r="L14">
-        <v>-12000</v>
+        <v>-1438</v>
       </c>
       <c r="M14">
-        <v>-700</v>
+        <v>-1366</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="A15" s="1">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B15" s="2">
         <v>44644</v>
@@ -1164,39 +1407,39 @@
         <v>13</v>
       </c>
       <c r="E15" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F15" s="2">
         <v>44686</v>
       </c>
       <c r="G15">
-        <v>0.001</v>
+        <v>0.008999999999999999</v>
       </c>
       <c r="H15">
-        <v>24.88</v>
+        <v>9.119999999999999</v>
       </c>
       <c r="I15" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J15" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="K15" t="s">
-        <v>51</v>
+        <v>82</v>
       </c>
       <c r="L15">
-        <v>-9024</v>
+        <v>-2200</v>
       </c>
       <c r="M15">
-        <v>-500</v>
+        <v>-2200</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="A16" s="1">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B16" s="2">
-        <v>44650</v>
+        <v>44657</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
@@ -1205,162 +1448,162 @@
         <v>13</v>
       </c>
       <c r="E16" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F16" s="2">
-        <v>44692</v>
+        <v>44699</v>
       </c>
       <c r="G16">
-        <v>0.0293</v>
+        <v>0.0065</v>
       </c>
       <c r="H16">
-        <v>10.11</v>
+        <v>9.58</v>
       </c>
       <c r="I16" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J16" t="s">
         <v>29</v>
       </c>
       <c r="K16" t="s">
-        <v>52</v>
+        <v>83</v>
       </c>
       <c r="L16">
-        <v>-1991</v>
+        <v>-6521</v>
       </c>
       <c r="M16">
-        <v>-1991</v>
+        <v>-1800</v>
       </c>
     </row>
     <row r="17" spans="1:13">
       <c r="A17" s="1">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="B17" s="2">
-        <v>44638</v>
+        <v>44649</v>
       </c>
       <c r="C17" t="s">
         <v>12</v>
       </c>
       <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F17" s="2">
+        <v>44691</v>
+      </c>
+      <c r="G17">
+        <v>0.0302</v>
+      </c>
+      <c r="H17">
         <v>14</v>
       </c>
-      <c r="E17" t="s">
-        <v>15</v>
-      </c>
-      <c r="F17" s="2">
-        <v>44680</v>
-      </c>
-      <c r="G17">
-        <v>0.7</v>
-      </c>
-      <c r="H17">
-        <v>5.31</v>
-      </c>
       <c r="I17" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J17" t="s">
         <v>30</v>
       </c>
       <c r="K17" t="s">
-        <v>53</v>
+        <v>84</v>
       </c>
       <c r="L17">
-        <v>-4200</v>
+        <v>-1908</v>
       </c>
       <c r="M17">
-        <v>-4200</v>
+        <v>-1908</v>
       </c>
     </row>
     <row r="18" spans="1:13">
       <c r="A18" s="1">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B18" s="2">
-        <v>44642</v>
+        <v>44651</v>
       </c>
       <c r="C18" t="s">
         <v>12</v>
       </c>
       <c r="D18" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E18" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F18" s="2">
-        <v>44684</v>
+        <v>44693</v>
       </c>
       <c r="G18">
-        <v>0.4</v>
+        <v>0.0303</v>
       </c>
       <c r="H18">
-        <v>5.77</v>
+        <v>13.68</v>
       </c>
       <c r="I18" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J18" t="s">
         <v>30</v>
       </c>
       <c r="K18" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="L18">
-        <v>-10300</v>
+        <v>-1900</v>
       </c>
       <c r="M18">
-        <v>-10300</v>
+        <v>-1900</v>
       </c>
     </row>
     <row r="19" spans="1:13">
       <c r="A19" s="1">
-        <v>24</v>
+        <v>19</v>
       </c>
       <c r="B19" s="2">
-        <v>44645</v>
+        <v>44651</v>
       </c>
       <c r="C19" t="s">
         <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E19" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F19" s="2">
-        <v>44687</v>
+        <v>44693</v>
       </c>
       <c r="G19">
-        <v>0.25</v>
+        <v>0.0303</v>
       </c>
       <c r="H19">
-        <v>6.37</v>
+        <v>13.68</v>
       </c>
       <c r="I19" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J19" t="s">
         <v>30</v>
       </c>
       <c r="K19" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
       <c r="L19">
-        <v>-15500</v>
+        <v>-7800</v>
       </c>
       <c r="M19">
-        <v>-7300</v>
+        <v>-1492</v>
       </c>
     </row>
     <row r="20" spans="1:13">
       <c r="A20" s="1">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B20" s="2">
-        <v>44650</v>
+        <v>44651</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
@@ -1369,39 +1612,39 @@
         <v>13</v>
       </c>
       <c r="E20" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F20" s="2">
-        <v>44692</v>
+        <v>44693</v>
       </c>
       <c r="G20">
-        <v>0.0015</v>
+        <v>0.0128</v>
       </c>
       <c r="H20">
-        <v>21.26</v>
+        <v>2.99</v>
       </c>
       <c r="I20" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J20" t="s">
         <v>31</v>
       </c>
       <c r="K20" t="s">
-        <v>56</v>
+        <v>87</v>
       </c>
       <c r="L20">
-        <v>-8077</v>
+        <v>-11911</v>
       </c>
       <c r="M20">
-        <v>-200</v>
+        <v>-5400</v>
       </c>
     </row>
     <row r="21" spans="1:13">
       <c r="A21" s="1">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B21" s="2">
-        <v>44649</v>
+        <v>44650</v>
       </c>
       <c r="C21" t="s">
         <v>12</v>
@@ -1410,39 +1653,39 @@
         <v>13</v>
       </c>
       <c r="E21" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F21" s="2">
-        <v>44691</v>
+        <v>44692</v>
       </c>
       <c r="G21">
-        <v>0.0335</v>
+        <v>0.0016</v>
       </c>
       <c r="H21">
-        <v>24.47</v>
+        <v>14.7</v>
       </c>
       <c r="I21" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J21" t="s">
         <v>32</v>
       </c>
       <c r="K21" t="s">
-        <v>57</v>
+        <v>88</v>
       </c>
       <c r="L21">
-        <v>-198</v>
+        <v>-12195</v>
       </c>
       <c r="M21">
-        <v>-198</v>
+        <v>-12195</v>
       </c>
     </row>
     <row r="22" spans="1:13">
       <c r="A22" s="1">
-        <v>28</v>
+        <v>22</v>
       </c>
       <c r="B22" s="2">
-        <v>44650</v>
+        <v>44657</v>
       </c>
       <c r="C22" t="s">
         <v>12</v>
@@ -1451,39 +1694,39 @@
         <v>13</v>
       </c>
       <c r="E22" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F22" s="2">
-        <v>44692</v>
+        <v>44699</v>
       </c>
       <c r="G22">
-        <v>0.0319</v>
+        <v>0.0189</v>
       </c>
       <c r="H22">
-        <v>25.14</v>
+        <v>6.04</v>
       </c>
       <c r="I22" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J22" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="K22" t="s">
-        <v>58</v>
+        <v>89</v>
       </c>
       <c r="L22">
-        <v>-2500</v>
+        <v>-11746</v>
       </c>
       <c r="M22">
-        <v>-2</v>
+        <v>-5400</v>
       </c>
     </row>
     <row r="23" spans="1:13">
       <c r="A23" s="1">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="B23" s="2">
-        <v>44651</v>
+        <v>44650</v>
       </c>
       <c r="C23" t="s">
         <v>12</v>
@@ -1492,39 +1735,39 @@
         <v>13</v>
       </c>
       <c r="E23" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F23" s="2">
-        <v>44693</v>
+        <v>44692</v>
       </c>
       <c r="G23">
-        <v>0.0173</v>
+        <v>0.0551</v>
       </c>
       <c r="H23">
-        <v>18.86</v>
+        <v>2.91</v>
       </c>
       <c r="I23" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J23" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="K23" t="s">
-        <v>59</v>
+        <v>90</v>
       </c>
       <c r="L23">
-        <v>-4833</v>
+        <v>-17000</v>
       </c>
       <c r="M23">
-        <v>-1300</v>
+        <v>-8700</v>
       </c>
     </row>
     <row r="24" spans="1:13">
       <c r="A24" s="1">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B24" s="2">
-        <v>44650</v>
+        <v>44649</v>
       </c>
       <c r="C24" t="s">
         <v>12</v>
@@ -1533,39 +1776,39 @@
         <v>13</v>
       </c>
       <c r="E24" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F24" s="2">
-        <v>44692</v>
+        <v>44691</v>
       </c>
       <c r="G24">
-        <v>0.0598</v>
+        <v>0.0083</v>
       </c>
       <c r="H24">
-        <v>16.78</v>
+        <v>7.35</v>
       </c>
       <c r="I24" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="K24" t="s">
-        <v>60</v>
+        <v>91</v>
       </c>
       <c r="L24">
-        <v>-1021</v>
+        <v>-2606</v>
       </c>
       <c r="M24">
-        <v>-200</v>
+        <v>-2606</v>
       </c>
     </row>
     <row r="25" spans="1:13">
       <c r="A25" s="1">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="B25" s="2">
-        <v>44649</v>
+        <v>44657</v>
       </c>
       <c r="C25" t="s">
         <v>12</v>
@@ -1574,36 +1817,36 @@
         <v>13</v>
       </c>
       <c r="E25" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F25" s="2">
-        <v>44691</v>
+        <v>44699</v>
       </c>
       <c r="G25">
-        <v>0.0016</v>
+        <v>0.0068</v>
       </c>
       <c r="H25">
-        <v>57.28</v>
+        <v>7.5</v>
       </c>
       <c r="I25" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J25" t="s">
         <v>35</v>
       </c>
       <c r="K25" t="s">
-        <v>61</v>
+        <v>92</v>
       </c>
       <c r="L25">
-        <v>-1406</v>
+        <v>-13600</v>
       </c>
       <c r="M25">
-        <v>-1406</v>
+        <v>-4894</v>
       </c>
     </row>
     <row r="26" spans="1:13">
       <c r="A26" s="1">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B26" s="2">
         <v>44650</v>
@@ -1615,7 +1858,7 @@
         <v>13</v>
       </c>
       <c r="E26" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F26" s="2">
         <v>44692</v>
@@ -1624,30 +1867,30 @@
         <v>0.0016</v>
       </c>
       <c r="H26">
-        <v>57.01</v>
+        <v>24.42</v>
       </c>
       <c r="I26" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J26" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="K26" t="s">
-        <v>62</v>
+        <v>93</v>
       </c>
       <c r="L26">
-        <v>-200</v>
+        <v>-3892</v>
       </c>
       <c r="M26">
-        <v>-200</v>
+        <v>-3892</v>
       </c>
     </row>
     <row r="27" spans="1:13">
       <c r="A27" s="1">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B27" s="2">
-        <v>44650</v>
+        <v>44644</v>
       </c>
       <c r="C27" t="s">
         <v>12</v>
@@ -1656,39 +1899,39 @@
         <v>13</v>
       </c>
       <c r="E27" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F27" s="2">
-        <v>44692</v>
+        <v>44686</v>
       </c>
       <c r="G27">
-        <v>0.0068</v>
+        <v>0.0016</v>
       </c>
       <c r="H27">
-        <v>24.48</v>
+        <v>23.71</v>
       </c>
       <c r="I27" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J27" t="s">
         <v>36</v>
       </c>
       <c r="K27" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="L27">
-        <v>-3650</v>
+        <v>-8156</v>
       </c>
       <c r="M27">
-        <v>-3650</v>
+        <v>-2308</v>
       </c>
     </row>
     <row r="28" spans="1:13">
       <c r="A28" s="1">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="B28" s="2">
-        <v>44644</v>
+        <v>44650</v>
       </c>
       <c r="C28" t="s">
         <v>12</v>
@@ -1697,72 +1940,2122 @@
         <v>13</v>
       </c>
       <c r="E28" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="F28" s="2">
-        <v>44686</v>
+        <v>44692</v>
       </c>
       <c r="G28">
-        <v>0.0057</v>
+        <v>0.0002</v>
       </c>
       <c r="H28">
-        <v>23.98</v>
+        <v>26.03</v>
       </c>
       <c r="I28" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="J28" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K28" t="s">
-        <v>64</v>
+        <v>95</v>
       </c>
       <c r="L28">
-        <v>-8779</v>
+        <v>-6000</v>
       </c>
       <c r="M28">
-        <v>-150</v>
+        <v>-6000</v>
       </c>
     </row>
     <row r="29" spans="1:13">
       <c r="A29" s="1">
+        <v>30</v>
+      </c>
+      <c r="B29" s="2">
+        <v>44649</v>
+      </c>
+      <c r="C29" t="s">
+        <v>12</v>
+      </c>
+      <c r="D29" t="s">
+        <v>13</v>
+      </c>
+      <c r="E29" t="s">
+        <v>18</v>
+      </c>
+      <c r="F29" s="2">
+        <v>44691</v>
+      </c>
+      <c r="G29">
+        <v>0.0635</v>
+      </c>
+      <c r="H29">
+        <v>15.87</v>
+      </c>
+      <c r="I29" t="s">
+        <v>19</v>
+      </c>
+      <c r="J29" t="s">
+        <v>38</v>
+      </c>
+      <c r="K29" t="s">
+        <v>96</v>
+      </c>
+      <c r="L29">
+        <v>-1515</v>
+      </c>
+      <c r="M29">
+        <v>-1515</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13">
+      <c r="A30" s="1">
+        <v>31</v>
+      </c>
+      <c r="B30" s="2">
+        <v>44644</v>
+      </c>
+      <c r="C30" t="s">
+        <v>12</v>
+      </c>
+      <c r="D30" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" t="s">
+        <v>18</v>
+      </c>
+      <c r="F30" s="2">
+        <v>44686</v>
+      </c>
+      <c r="G30">
+        <v>0.06809999999999999</v>
+      </c>
+      <c r="H30">
+        <v>14.31</v>
+      </c>
+      <c r="I30" t="s">
+        <v>19</v>
+      </c>
+      <c r="J30" t="s">
+        <v>38</v>
+      </c>
+      <c r="K30" t="s">
+        <v>97</v>
+      </c>
+      <c r="L30">
+        <v>-23200</v>
+      </c>
+      <c r="M30">
+        <v>-18385</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13">
+      <c r="A31" s="1">
+        <v>32</v>
+      </c>
+      <c r="B31" s="2">
+        <v>44657</v>
+      </c>
+      <c r="C31" t="s">
+        <v>12</v>
+      </c>
+      <c r="D31" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" t="s">
+        <v>18</v>
+      </c>
+      <c r="F31" s="2">
+        <v>44699</v>
+      </c>
+      <c r="G31">
+        <v>0.1081</v>
+      </c>
+      <c r="H31">
+        <v>14.44</v>
+      </c>
+      <c r="I31" t="s">
+        <v>19</v>
+      </c>
+      <c r="J31" t="s">
+        <v>39</v>
+      </c>
+      <c r="K31" t="s">
+        <v>98</v>
+      </c>
+      <c r="L31">
+        <v>-3091</v>
+      </c>
+      <c r="M31">
+        <v>-1400</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13">
+      <c r="A32" s="1">
+        <v>33</v>
+      </c>
+      <c r="B32" s="2">
+        <v>44650</v>
+      </c>
+      <c r="C32" t="s">
+        <v>12</v>
+      </c>
+      <c r="D32" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" t="s">
+        <v>18</v>
+      </c>
+      <c r="F32" s="2">
+        <v>44692</v>
+      </c>
+      <c r="G32">
+        <v>0.0089</v>
+      </c>
+      <c r="H32">
+        <v>43.37</v>
+      </c>
+      <c r="I32" t="s">
+        <v>19</v>
+      </c>
+      <c r="J32" t="s">
+        <v>40</v>
+      </c>
+      <c r="K32" t="s">
+        <v>99</v>
+      </c>
+      <c r="L32">
+        <v>-2400</v>
+      </c>
+      <c r="M32">
+        <v>-1400</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13">
+      <c r="A33" s="1">
+        <v>35</v>
+      </c>
+      <c r="B33" s="2">
+        <v>44657</v>
+      </c>
+      <c r="C33" t="s">
+        <v>12</v>
+      </c>
+      <c r="D33" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" t="s">
+        <v>18</v>
+      </c>
+      <c r="F33" s="2">
+        <v>44699</v>
+      </c>
+      <c r="G33">
+        <v>0.0056</v>
+      </c>
+      <c r="H33">
+        <v>37.93</v>
+      </c>
+      <c r="I33" t="s">
+        <v>19</v>
+      </c>
+      <c r="J33" t="s">
+        <v>41</v>
+      </c>
+      <c r="K33" t="s">
+        <v>100</v>
+      </c>
+      <c r="L33">
+        <v>-916</v>
+      </c>
+      <c r="M33">
+        <v>-916</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13">
+      <c r="A34" s="1">
+        <v>36</v>
+      </c>
+      <c r="B34" s="2">
+        <v>44644</v>
+      </c>
+      <c r="C34" t="s">
+        <v>12</v>
+      </c>
+      <c r="D34" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" t="s">
+        <v>18</v>
+      </c>
+      <c r="F34" s="2">
+        <v>44686</v>
+      </c>
+      <c r="G34">
+        <v>0.0054</v>
+      </c>
+      <c r="H34">
+        <v>35.64</v>
+      </c>
+      <c r="I34" t="s">
+        <v>19</v>
+      </c>
+      <c r="J34" t="s">
+        <v>41</v>
+      </c>
+      <c r="K34" t="s">
+        <v>101</v>
+      </c>
+      <c r="L34">
+        <v>-1647</v>
+      </c>
+      <c r="M34">
+        <v>-284</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13">
+      <c r="A35" s="1">
         <v>37</v>
       </c>
-      <c r="B29" s="2">
+      <c r="B35" s="2">
+        <v>44657</v>
+      </c>
+      <c r="C35" t="s">
+        <v>12</v>
+      </c>
+      <c r="D35" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" t="s">
+        <v>18</v>
+      </c>
+      <c r="F35" s="2">
+        <v>44699</v>
+      </c>
+      <c r="G35">
+        <v>0.0207</v>
+      </c>
+      <c r="H35">
+        <v>24.1</v>
+      </c>
+      <c r="I35" t="s">
+        <v>19</v>
+      </c>
+      <c r="J35" t="s">
+        <v>42</v>
+      </c>
+      <c r="K35" t="s">
+        <v>102</v>
+      </c>
+      <c r="L35">
+        <v>-2503</v>
+      </c>
+      <c r="M35">
+        <v>-1100</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13">
+      <c r="A36" s="1">
+        <v>38</v>
+      </c>
+      <c r="B36" s="2">
+        <v>44644</v>
+      </c>
+      <c r="C36" t="s">
+        <v>12</v>
+      </c>
+      <c r="D36" t="s">
+        <v>13</v>
+      </c>
+      <c r="E36" t="s">
+        <v>18</v>
+      </c>
+      <c r="F36" s="2">
+        <v>44686</v>
+      </c>
+      <c r="G36">
+        <v>0.003</v>
+      </c>
+      <c r="H36">
+        <v>27.06</v>
+      </c>
+      <c r="I36" t="s">
+        <v>19</v>
+      </c>
+      <c r="J36" t="s">
+        <v>43</v>
+      </c>
+      <c r="K36" t="s">
+        <v>103</v>
+      </c>
+      <c r="L36">
+        <v>-8703</v>
+      </c>
+      <c r="M36">
+        <v>-6000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13">
+      <c r="A37" s="1">
+        <v>40</v>
+      </c>
+      <c r="B37" s="2">
+        <v>44657</v>
+      </c>
+      <c r="C37" t="s">
+        <v>12</v>
+      </c>
+      <c r="D37" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" t="s">
+        <v>18</v>
+      </c>
+      <c r="F37" s="2">
+        <v>44699</v>
+      </c>
+      <c r="G37">
+        <v>0.0444</v>
+      </c>
+      <c r="H37">
+        <v>18.89</v>
+      </c>
+      <c r="I37" t="s">
+        <v>19</v>
+      </c>
+      <c r="J37" t="s">
+        <v>44</v>
+      </c>
+      <c r="K37" t="s">
+        <v>104</v>
+      </c>
+      <c r="L37">
+        <v>-65</v>
+      </c>
+      <c r="M37">
+        <v>-65</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13">
+      <c r="A38" s="1">
+        <v>41</v>
+      </c>
+      <c r="B38" s="2">
+        <v>44651</v>
+      </c>
+      <c r="C38" t="s">
+        <v>12</v>
+      </c>
+      <c r="D38" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" t="s">
+        <v>18</v>
+      </c>
+      <c r="F38" s="2">
+        <v>44693</v>
+      </c>
+      <c r="G38">
+        <v>0.0279</v>
+      </c>
+      <c r="H38">
+        <v>30.48</v>
+      </c>
+      <c r="I38" t="s">
+        <v>19</v>
+      </c>
+      <c r="J38" t="s">
+        <v>45</v>
+      </c>
+      <c r="K38" t="s">
+        <v>105</v>
+      </c>
+      <c r="L38">
+        <v>-15000</v>
+      </c>
+      <c r="M38">
+        <v>-5200</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13">
+      <c r="A39" s="1">
+        <v>43</v>
+      </c>
+      <c r="B39" s="2">
         <v>44650</v>
       </c>
-      <c r="C29" t="s">
-        <v>12</v>
-      </c>
-      <c r="D29" t="s">
-        <v>13</v>
-      </c>
-      <c r="E29" t="s">
+      <c r="C39" t="s">
+        <v>12</v>
+      </c>
+      <c r="D39" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" t="s">
+        <v>18</v>
+      </c>
+      <c r="F39" s="2">
+        <v>44692</v>
+      </c>
+      <c r="G39">
+        <v>0.1866</v>
+      </c>
+      <c r="H39">
+        <v>17.73</v>
+      </c>
+      <c r="I39" t="s">
+        <v>19</v>
+      </c>
+      <c r="J39" t="s">
+        <v>46</v>
+      </c>
+      <c r="K39" t="s">
+        <v>106</v>
+      </c>
+      <c r="L39">
+        <v>-1600</v>
+      </c>
+      <c r="M39">
+        <v>-900</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13">
+      <c r="A40" s="1">
+        <v>45</v>
+      </c>
+      <c r="B40" s="2">
+        <v>44657</v>
+      </c>
+      <c r="C40" t="s">
+        <v>12</v>
+      </c>
+      <c r="D40" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" t="s">
+        <v>18</v>
+      </c>
+      <c r="F40" s="2">
+        <v>44699</v>
+      </c>
+      <c r="G40">
+        <v>0.0055</v>
+      </c>
+      <c r="H40">
+        <v>39.35</v>
+      </c>
+      <c r="I40" t="s">
+        <v>19</v>
+      </c>
+      <c r="J40" t="s">
+        <v>47</v>
+      </c>
+      <c r="K40" t="s">
+        <v>107</v>
+      </c>
+      <c r="L40">
+        <v>-4139</v>
+      </c>
+      <c r="M40">
+        <v>-1900</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13">
+      <c r="A41" s="1">
+        <v>46</v>
+      </c>
+      <c r="B41" s="2">
+        <v>44651</v>
+      </c>
+      <c r="C41" t="s">
+        <v>12</v>
+      </c>
+      <c r="D41" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" t="s">
+        <v>18</v>
+      </c>
+      <c r="F41" s="2">
+        <v>44693</v>
+      </c>
+      <c r="G41">
+        <v>0.0019</v>
+      </c>
+      <c r="H41">
+        <v>27.7</v>
+      </c>
+      <c r="I41" t="s">
+        <v>19</v>
+      </c>
+      <c r="J41" t="s">
+        <v>48</v>
+      </c>
+      <c r="K41" t="s">
+        <v>108</v>
+      </c>
+      <c r="L41">
+        <v>-8928</v>
+      </c>
+      <c r="M41">
+        <v>-8928</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13">
+      <c r="A42" s="1">
+        <v>47</v>
+      </c>
+      <c r="B42" s="2">
+        <v>44652</v>
+      </c>
+      <c r="C42" t="s">
+        <v>12</v>
+      </c>
+      <c r="D42" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" t="s">
+        <v>18</v>
+      </c>
+      <c r="F42" s="2">
+        <v>44694</v>
+      </c>
+      <c r="G42">
+        <v>0.0019</v>
+      </c>
+      <c r="H42">
+        <v>27.62</v>
+      </c>
+      <c r="I42" t="s">
+        <v>19</v>
+      </c>
+      <c r="J42" t="s">
+        <v>48</v>
+      </c>
+      <c r="K42" t="s">
+        <v>109</v>
+      </c>
+      <c r="L42">
+        <v>-8000</v>
+      </c>
+      <c r="M42">
+        <v>-8000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13">
+      <c r="A43" s="1">
+        <v>48</v>
+      </c>
+      <c r="B43" s="2">
+        <v>44657</v>
+      </c>
+      <c r="C43" t="s">
+        <v>12</v>
+      </c>
+      <c r="D43" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" t="s">
+        <v>18</v>
+      </c>
+      <c r="F43" s="2">
+        <v>44699</v>
+      </c>
+      <c r="G43">
+        <v>0.0016</v>
+      </c>
+      <c r="H43">
+        <v>26.83</v>
+      </c>
+      <c r="I43" t="s">
+        <v>19</v>
+      </c>
+      <c r="J43" t="s">
+        <v>48</v>
+      </c>
+      <c r="K43" t="s">
+        <v>110</v>
+      </c>
+      <c r="L43">
+        <v>-32844</v>
+      </c>
+      <c r="M43">
+        <v>-5872</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13">
+      <c r="A44" s="1">
+        <v>49</v>
+      </c>
+      <c r="B44" s="2">
+        <v>44657</v>
+      </c>
+      <c r="C44" t="s">
+        <v>12</v>
+      </c>
+      <c r="D44" t="s">
+        <v>13</v>
+      </c>
+      <c r="E44" t="s">
+        <v>18</v>
+      </c>
+      <c r="F44" s="2">
+        <v>44699</v>
+      </c>
+      <c r="G44">
+        <v>0.0116</v>
+      </c>
+      <c r="H44">
+        <v>6.75</v>
+      </c>
+      <c r="I44" t="s">
+        <v>19</v>
+      </c>
+      <c r="J44" t="s">
+        <v>49</v>
+      </c>
+      <c r="K44" t="s">
+        <v>111</v>
+      </c>
+      <c r="L44">
+        <v>-610</v>
+      </c>
+      <c r="M44">
+        <v>-610</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13">
+      <c r="A45" s="1">
+        <v>50</v>
+      </c>
+      <c r="B45" s="2">
+        <v>44651</v>
+      </c>
+      <c r="C45" t="s">
+        <v>12</v>
+      </c>
+      <c r="D45" t="s">
+        <v>13</v>
+      </c>
+      <c r="E45" t="s">
+        <v>18</v>
+      </c>
+      <c r="F45" s="2">
+        <v>44693</v>
+      </c>
+      <c r="G45">
+        <v>0.0056</v>
+      </c>
+      <c r="H45">
+        <v>6.6</v>
+      </c>
+      <c r="I45" t="s">
+        <v>19</v>
+      </c>
+      <c r="J45" t="s">
+        <v>49</v>
+      </c>
+      <c r="K45" t="s">
+        <v>112</v>
+      </c>
+      <c r="L45">
+        <v>-2700</v>
+      </c>
+      <c r="M45">
+        <v>-790</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13">
+      <c r="A46" s="1">
+        <v>51</v>
+      </c>
+      <c r="B46" s="2">
+        <v>44651</v>
+      </c>
+      <c r="C46" t="s">
+        <v>12</v>
+      </c>
+      <c r="D46" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46" t="s">
+        <v>18</v>
+      </c>
+      <c r="F46" s="2">
+        <v>44693</v>
+      </c>
+      <c r="G46">
+        <v>0.0023</v>
+      </c>
+      <c r="H46">
+        <v>26.97</v>
+      </c>
+      <c r="I46" t="s">
+        <v>19</v>
+      </c>
+      <c r="J46" t="s">
+        <v>50</v>
+      </c>
+      <c r="K46" t="s">
+        <v>113</v>
+      </c>
+      <c r="L46">
+        <v>-3477</v>
+      </c>
+      <c r="M46">
+        <v>-1500</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13">
+      <c r="A47" s="1">
+        <v>52</v>
+      </c>
+      <c r="B47" s="2">
+        <v>44644</v>
+      </c>
+      <c r="C47" t="s">
+        <v>12</v>
+      </c>
+      <c r="D47" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" t="s">
+        <v>18</v>
+      </c>
+      <c r="F47" s="2">
+        <v>44686</v>
+      </c>
+      <c r="G47">
+        <v>0.001</v>
+      </c>
+      <c r="H47">
+        <v>24.88</v>
+      </c>
+      <c r="I47" t="s">
+        <v>19</v>
+      </c>
+      <c r="J47" t="s">
+        <v>51</v>
+      </c>
+      <c r="K47" t="s">
+        <v>114</v>
+      </c>
+      <c r="L47">
+        <v>-9024</v>
+      </c>
+      <c r="M47">
+        <v>-5200</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13">
+      <c r="A48" s="1">
+        <v>54</v>
+      </c>
+      <c r="B48" s="2">
+        <v>44638</v>
+      </c>
+      <c r="C48" t="s">
+        <v>12</v>
+      </c>
+      <c r="D48" t="s">
         <v>15</v>
       </c>
-      <c r="F29" s="2">
+      <c r="E48" t="s">
+        <v>18</v>
+      </c>
+      <c r="F48" s="2">
+        <v>44680</v>
+      </c>
+      <c r="G48">
+        <v>0.7</v>
+      </c>
+      <c r="H48">
+        <v>5.31</v>
+      </c>
+      <c r="I48" t="s">
+        <v>19</v>
+      </c>
+      <c r="J48" t="s">
+        <v>52</v>
+      </c>
+      <c r="K48" t="s">
+        <v>115</v>
+      </c>
+      <c r="L48">
+        <v>-4200</v>
+      </c>
+      <c r="M48">
+        <v>-4200</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13">
+      <c r="A49" s="1">
+        <v>55</v>
+      </c>
+      <c r="B49" s="2">
+        <v>44642</v>
+      </c>
+      <c r="C49" t="s">
+        <v>12</v>
+      </c>
+      <c r="D49" t="s">
+        <v>15</v>
+      </c>
+      <c r="E49" t="s">
+        <v>18</v>
+      </c>
+      <c r="F49" s="2">
+        <v>44684</v>
+      </c>
+      <c r="G49">
+        <v>0.4</v>
+      </c>
+      <c r="H49">
+        <v>5.77</v>
+      </c>
+      <c r="I49" t="s">
+        <v>19</v>
+      </c>
+      <c r="J49" t="s">
+        <v>52</v>
+      </c>
+      <c r="K49" t="s">
+        <v>116</v>
+      </c>
+      <c r="L49">
+        <v>-10300</v>
+      </c>
+      <c r="M49">
+        <v>-10300</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13">
+      <c r="A50" s="1">
+        <v>56</v>
+      </c>
+      <c r="B50" s="2">
+        <v>44645</v>
+      </c>
+      <c r="C50" t="s">
+        <v>12</v>
+      </c>
+      <c r="D50" t="s">
+        <v>15</v>
+      </c>
+      <c r="E50" t="s">
+        <v>18</v>
+      </c>
+      <c r="F50" s="2">
+        <v>44687</v>
+      </c>
+      <c r="G50">
+        <v>0.25</v>
+      </c>
+      <c r="H50">
+        <v>6.37</v>
+      </c>
+      <c r="I50" t="s">
+        <v>19</v>
+      </c>
+      <c r="J50" t="s">
+        <v>52</v>
+      </c>
+      <c r="K50" t="s">
+        <v>117</v>
+      </c>
+      <c r="L50">
+        <v>-15500</v>
+      </c>
+      <c r="M50">
+        <v>-15500</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13">
+      <c r="A51" s="1">
+        <v>57</v>
+      </c>
+      <c r="B51" s="2">
+        <v>44651</v>
+      </c>
+      <c r="C51" t="s">
+        <v>12</v>
+      </c>
+      <c r="D51" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" t="s">
+        <v>18</v>
+      </c>
+      <c r="F51" s="2">
+        <v>44693</v>
+      </c>
+      <c r="G51">
+        <v>0.09</v>
+      </c>
+      <c r="H51">
+        <v>6.93</v>
+      </c>
+      <c r="I51" t="s">
+        <v>19</v>
+      </c>
+      <c r="J51" t="s">
+        <v>52</v>
+      </c>
+      <c r="K51" t="s">
+        <v>118</v>
+      </c>
+      <c r="L51">
+        <v>-244374</v>
+      </c>
+      <c r="M51">
+        <v>-10600</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13">
+      <c r="A52" s="1">
+        <v>58</v>
+      </c>
+      <c r="B52" s="2">
+        <v>44650</v>
+      </c>
+      <c r="C52" t="s">
+        <v>12</v>
+      </c>
+      <c r="D52" t="s">
+        <v>13</v>
+      </c>
+      <c r="E52" t="s">
+        <v>18</v>
+      </c>
+      <c r="F52" s="2">
         <v>44692</v>
       </c>
-      <c r="G29">
-        <v>0.003</v>
-      </c>
-      <c r="H29">
-        <v>34.09</v>
-      </c>
-      <c r="I29" t="s">
-        <v>16</v>
-      </c>
-      <c r="J29" t="s">
-        <v>37</v>
-      </c>
-      <c r="K29" t="s">
+      <c r="G52">
+        <v>0.0015</v>
+      </c>
+      <c r="H52">
+        <v>21.26</v>
+      </c>
+      <c r="I52" t="s">
+        <v>19</v>
+      </c>
+      <c r="J52" t="s">
+        <v>53</v>
+      </c>
+      <c r="K52" t="s">
+        <v>119</v>
+      </c>
+      <c r="L52">
+        <v>-8077</v>
+      </c>
+      <c r="M52">
+        <v>-1900</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13">
+      <c r="A53" s="1">
+        <v>59</v>
+      </c>
+      <c r="B53" s="2">
+        <v>44657</v>
+      </c>
+      <c r="C53" t="s">
+        <v>12</v>
+      </c>
+      <c r="D53" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" t="s">
+        <v>18</v>
+      </c>
+      <c r="F53" s="2">
+        <v>44699</v>
+      </c>
+      <c r="G53">
+        <v>0.0021</v>
+      </c>
+      <c r="H53">
+        <v>12.44</v>
+      </c>
+      <c r="I53" t="s">
+        <v>19</v>
+      </c>
+      <c r="J53" t="s">
+        <v>54</v>
+      </c>
+      <c r="K53" t="s">
+        <v>120</v>
+      </c>
+      <c r="L53">
+        <v>-3036</v>
+      </c>
+      <c r="M53">
+        <v>-1400</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13">
+      <c r="A54" s="1">
+        <v>60</v>
+      </c>
+      <c r="B54" s="2">
+        <v>44649</v>
+      </c>
+      <c r="C54" t="s">
+        <v>12</v>
+      </c>
+      <c r="D54" t="s">
+        <v>13</v>
+      </c>
+      <c r="E54" t="s">
+        <v>18</v>
+      </c>
+      <c r="F54" s="2">
+        <v>44691</v>
+      </c>
+      <c r="G54">
+        <v>0.0335</v>
+      </c>
+      <c r="H54">
+        <v>24.47</v>
+      </c>
+      <c r="I54" t="s">
+        <v>19</v>
+      </c>
+      <c r="J54" t="s">
+        <v>55</v>
+      </c>
+      <c r="K54" t="s">
+        <v>121</v>
+      </c>
+      <c r="L54">
+        <v>-198</v>
+      </c>
+      <c r="M54">
+        <v>-198</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13">
+      <c r="A55" s="1">
+        <v>61</v>
+      </c>
+      <c r="B55" s="2">
+        <v>44650</v>
+      </c>
+      <c r="C55" t="s">
+        <v>12</v>
+      </c>
+      <c r="D55" t="s">
+        <v>13</v>
+      </c>
+      <c r="E55" t="s">
+        <v>18</v>
+      </c>
+      <c r="F55" s="2">
+        <v>44692</v>
+      </c>
+      <c r="G55">
+        <v>0.0319</v>
+      </c>
+      <c r="H55">
+        <v>25.14</v>
+      </c>
+      <c r="I55" t="s">
+        <v>19</v>
+      </c>
+      <c r="J55" t="s">
+        <v>55</v>
+      </c>
+      <c r="K55" t="s">
+        <v>122</v>
+      </c>
+      <c r="L55">
+        <v>-2500</v>
+      </c>
+      <c r="M55">
+        <v>-1302</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13">
+      <c r="A56" s="1">
+        <v>63</v>
+      </c>
+      <c r="B56" s="2">
+        <v>44657</v>
+      </c>
+      <c r="C56" t="s">
+        <v>12</v>
+      </c>
+      <c r="D56" t="s">
+        <v>13</v>
+      </c>
+      <c r="E56" t="s">
+        <v>18</v>
+      </c>
+      <c r="F56" s="2">
+        <v>44699</v>
+      </c>
+      <c r="G56">
+        <v>0.0011</v>
+      </c>
+      <c r="H56">
+        <v>28.04</v>
+      </c>
+      <c r="I56" t="s">
+        <v>19</v>
+      </c>
+      <c r="J56" t="s">
+        <v>56</v>
+      </c>
+      <c r="K56" t="s">
+        <v>123</v>
+      </c>
+      <c r="L56">
+        <v>-10014</v>
+      </c>
+      <c r="M56">
+        <v>-4000</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13">
+      <c r="A57" s="1">
         <v>65</v>
       </c>
-      <c r="L29">
-        <v>-5181</v>
-      </c>
-      <c r="M29">
-        <v>-800</v>
+      <c r="B57" s="2">
+        <v>44656</v>
+      </c>
+      <c r="C57" t="s">
+        <v>12</v>
+      </c>
+      <c r="D57" t="s">
+        <v>17</v>
+      </c>
+      <c r="E57" t="s">
+        <v>18</v>
+      </c>
+      <c r="F57" s="2">
+        <v>44698</v>
+      </c>
+      <c r="G57">
+        <v>0.0005999999999999999</v>
+      </c>
+      <c r="H57">
+        <v>34.69</v>
+      </c>
+      <c r="I57" t="s">
+        <v>19</v>
+      </c>
+      <c r="J57" t="s">
+        <v>57</v>
+      </c>
+      <c r="K57" t="s">
+        <v>124</v>
+      </c>
+      <c r="L57">
+        <v>-2000</v>
+      </c>
+      <c r="M57">
+        <v>-2000</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13">
+      <c r="A58" s="1">
+        <v>66</v>
+      </c>
+      <c r="B58" s="2">
+        <v>44656</v>
+      </c>
+      <c r="C58" t="s">
+        <v>12</v>
+      </c>
+      <c r="D58" t="s">
+        <v>15</v>
+      </c>
+      <c r="E58" t="s">
+        <v>18</v>
+      </c>
+      <c r="F58" s="2">
+        <v>44698</v>
+      </c>
+      <c r="G58">
+        <v>0.0005999999999999999</v>
+      </c>
+      <c r="H58">
+        <v>34.69</v>
+      </c>
+      <c r="I58" t="s">
+        <v>19</v>
+      </c>
+      <c r="J58" t="s">
+        <v>57</v>
+      </c>
+      <c r="K58" t="s">
+        <v>125</v>
+      </c>
+      <c r="L58">
+        <v>-4700</v>
+      </c>
+      <c r="M58">
+        <v>-4700</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13">
+      <c r="A59" s="1">
+        <v>67</v>
+      </c>
+      <c r="B59" s="2">
+        <v>44656</v>
+      </c>
+      <c r="C59" t="s">
+        <v>12</v>
+      </c>
+      <c r="D59" t="s">
+        <v>15</v>
+      </c>
+      <c r="E59" t="s">
+        <v>18</v>
+      </c>
+      <c r="F59" s="2">
+        <v>44698</v>
+      </c>
+      <c r="G59">
+        <v>0.0005999999999999999</v>
+      </c>
+      <c r="H59">
+        <v>34.69</v>
+      </c>
+      <c r="I59" t="s">
+        <v>19</v>
+      </c>
+      <c r="J59" t="s">
+        <v>57</v>
+      </c>
+      <c r="K59" t="s">
+        <v>126</v>
+      </c>
+      <c r="L59">
+        <v>-1124</v>
+      </c>
+      <c r="M59">
+        <v>-1124</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13">
+      <c r="A60" s="1">
+        <v>68</v>
+      </c>
+      <c r="B60" s="2">
+        <v>44657</v>
+      </c>
+      <c r="C60" t="s">
+        <v>12</v>
+      </c>
+      <c r="D60" t="s">
+        <v>13</v>
+      </c>
+      <c r="E60" t="s">
+        <v>18</v>
+      </c>
+      <c r="F60" s="2">
+        <v>44699</v>
+      </c>
+      <c r="G60">
+        <v>0.0005</v>
+      </c>
+      <c r="H60">
+        <v>35.03</v>
+      </c>
+      <c r="I60" t="s">
+        <v>19</v>
+      </c>
+      <c r="J60" t="s">
+        <v>57</v>
+      </c>
+      <c r="K60" t="s">
+        <v>127</v>
+      </c>
+      <c r="L60">
+        <v>-15600</v>
+      </c>
+      <c r="M60">
+        <v>-3000</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13">
+      <c r="A61" s="1">
+        <v>70</v>
+      </c>
+      <c r="B61" s="2">
+        <v>44656</v>
+      </c>
+      <c r="C61" t="s">
+        <v>12</v>
+      </c>
+      <c r="D61" t="s">
+        <v>17</v>
+      </c>
+      <c r="E61" t="s">
+        <v>18</v>
+      </c>
+      <c r="F61" s="2">
+        <v>44698</v>
+      </c>
+      <c r="G61">
+        <v>0.0003</v>
+      </c>
+      <c r="H61">
+        <v>32.59</v>
+      </c>
+      <c r="I61" t="s">
+        <v>19</v>
+      </c>
+      <c r="J61" t="s">
+        <v>58</v>
+      </c>
+      <c r="K61" t="s">
+        <v>128</v>
+      </c>
+      <c r="L61">
+        <v>-1100</v>
+      </c>
+      <c r="M61">
+        <v>-1100</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13">
+      <c r="A62" s="1">
+        <v>71</v>
+      </c>
+      <c r="B62" s="2">
+        <v>44657</v>
+      </c>
+      <c r="C62" t="s">
+        <v>12</v>
+      </c>
+      <c r="D62" t="s">
+        <v>13</v>
+      </c>
+      <c r="E62" t="s">
+        <v>18</v>
+      </c>
+      <c r="F62" s="2">
+        <v>44699</v>
+      </c>
+      <c r="G62">
+        <v>0.0002</v>
+      </c>
+      <c r="H62">
+        <v>32.62</v>
+      </c>
+      <c r="I62" t="s">
+        <v>19</v>
+      </c>
+      <c r="J62" t="s">
+        <v>58</v>
+      </c>
+      <c r="K62" t="s">
+        <v>129</v>
+      </c>
+      <c r="L62">
+        <v>-11200</v>
+      </c>
+      <c r="M62">
+        <v>-11200</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13">
+      <c r="A63" s="1">
+        <v>72</v>
+      </c>
+      <c r="B63" s="2">
+        <v>44657</v>
+      </c>
+      <c r="C63" t="s">
+        <v>12</v>
+      </c>
+      <c r="D63" t="s">
+        <v>13</v>
+      </c>
+      <c r="E63" t="s">
+        <v>18</v>
+      </c>
+      <c r="F63" s="2">
+        <v>44699</v>
+      </c>
+      <c r="G63">
+        <v>0.0002</v>
+      </c>
+      <c r="H63">
+        <v>32.62</v>
+      </c>
+      <c r="I63" t="s">
+        <v>19</v>
+      </c>
+      <c r="J63" t="s">
+        <v>58</v>
+      </c>
+      <c r="K63" t="s">
+        <v>130</v>
+      </c>
+      <c r="L63">
+        <v>-1649</v>
+      </c>
+      <c r="M63">
+        <v>-1649</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13">
+      <c r="A64" s="1">
+        <v>73</v>
+      </c>
+      <c r="B64" s="2">
+        <v>44657</v>
+      </c>
+      <c r="C64" t="s">
+        <v>12</v>
+      </c>
+      <c r="D64" t="s">
+        <v>13</v>
+      </c>
+      <c r="E64" t="s">
+        <v>18</v>
+      </c>
+      <c r="F64" s="2">
+        <v>44699</v>
+      </c>
+      <c r="G64">
+        <v>0.0484</v>
+      </c>
+      <c r="H64">
+        <v>9.279999999999999</v>
+      </c>
+      <c r="I64" t="s">
+        <v>19</v>
+      </c>
+      <c r="J64" t="s">
+        <v>59</v>
+      </c>
+      <c r="K64" t="s">
+        <v>131</v>
+      </c>
+      <c r="L64">
+        <v>-3835</v>
+      </c>
+      <c r="M64">
+        <v>-400</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13">
+      <c r="A65" s="1">
+        <v>74</v>
+      </c>
+      <c r="B65" s="2">
+        <v>44650</v>
+      </c>
+      <c r="C65" t="s">
+        <v>12</v>
+      </c>
+      <c r="D65" t="s">
+        <v>13</v>
+      </c>
+      <c r="E65" t="s">
+        <v>18</v>
+      </c>
+      <c r="F65" s="2">
+        <v>44692</v>
+      </c>
+      <c r="G65">
+        <v>0.0109</v>
+      </c>
+      <c r="H65">
+        <v>24.05</v>
+      </c>
+      <c r="I65" t="s">
+        <v>19</v>
+      </c>
+      <c r="J65" t="s">
+        <v>60</v>
+      </c>
+      <c r="K65" t="s">
+        <v>132</v>
+      </c>
+      <c r="L65">
+        <v>-10942</v>
+      </c>
+      <c r="M65">
+        <v>-4927</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13">
+      <c r="A66" s="1">
+        <v>75</v>
+      </c>
+      <c r="B66" s="2">
+        <v>44656</v>
+      </c>
+      <c r="C66" t="s">
+        <v>12</v>
+      </c>
+      <c r="D66" t="s">
+        <v>17</v>
+      </c>
+      <c r="E66" t="s">
+        <v>18</v>
+      </c>
+      <c r="F66" s="2">
+        <v>44698</v>
+      </c>
+      <c r="G66">
+        <v>0.0336</v>
+      </c>
+      <c r="H66">
+        <v>18.88</v>
+      </c>
+      <c r="I66" t="s">
+        <v>19</v>
+      </c>
+      <c r="J66" t="s">
+        <v>61</v>
+      </c>
+      <c r="K66" t="s">
+        <v>133</v>
+      </c>
+      <c r="L66">
+        <v>-500</v>
+      </c>
+      <c r="M66">
+        <v>-500</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13">
+      <c r="A67" s="1">
+        <v>76</v>
+      </c>
+      <c r="B67" s="2">
+        <v>44657</v>
+      </c>
+      <c r="C67" t="s">
+        <v>12</v>
+      </c>
+      <c r="D67" t="s">
+        <v>13</v>
+      </c>
+      <c r="E67" t="s">
+        <v>18</v>
+      </c>
+      <c r="F67" s="2">
+        <v>44699</v>
+      </c>
+      <c r="G67">
+        <v>0.0336</v>
+      </c>
+      <c r="H67">
+        <v>18.56</v>
+      </c>
+      <c r="I67" t="s">
+        <v>19</v>
+      </c>
+      <c r="J67" t="s">
+        <v>61</v>
+      </c>
+      <c r="K67" t="s">
+        <v>134</v>
+      </c>
+      <c r="L67">
+        <v>-12297</v>
+      </c>
+      <c r="M67">
+        <v>-5300</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13">
+      <c r="A68" s="1">
+        <v>77</v>
+      </c>
+      <c r="B68" s="2">
+        <v>44650</v>
+      </c>
+      <c r="C68" t="s">
+        <v>12</v>
+      </c>
+      <c r="D68" t="s">
+        <v>13</v>
+      </c>
+      <c r="E68" t="s">
+        <v>18</v>
+      </c>
+      <c r="F68" s="2">
+        <v>44692</v>
+      </c>
+      <c r="G68">
+        <v>0.0294</v>
+      </c>
+      <c r="H68">
+        <v>62.55</v>
+      </c>
+      <c r="I68" t="s">
+        <v>19</v>
+      </c>
+      <c r="J68" t="s">
+        <v>62</v>
+      </c>
+      <c r="K68" t="s">
+        <v>135</v>
+      </c>
+      <c r="L68">
+        <v>-5500</v>
+      </c>
+      <c r="M68">
+        <v>-1509</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13">
+      <c r="A69" s="1">
+        <v>79</v>
+      </c>
+      <c r="B69" s="2">
+        <v>44657</v>
+      </c>
+      <c r="C69" t="s">
+        <v>12</v>
+      </c>
+      <c r="D69" t="s">
+        <v>13</v>
+      </c>
+      <c r="E69" t="s">
+        <v>18</v>
+      </c>
+      <c r="F69" s="2">
+        <v>44699</v>
+      </c>
+      <c r="G69">
+        <v>0.06510000000000001</v>
+      </c>
+      <c r="H69">
+        <v>51.22</v>
+      </c>
+      <c r="I69" t="s">
+        <v>19</v>
+      </c>
+      <c r="J69" t="s">
+        <v>63</v>
+      </c>
+      <c r="K69" t="s">
+        <v>136</v>
+      </c>
+      <c r="L69">
+        <v>-3599</v>
+      </c>
+      <c r="M69">
+        <v>-1600</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13">
+      <c r="A70" s="1">
+        <v>80</v>
+      </c>
+      <c r="B70" s="2">
+        <v>44656</v>
+      </c>
+      <c r="C70" t="s">
+        <v>12</v>
+      </c>
+      <c r="D70" t="s">
+        <v>17</v>
+      </c>
+      <c r="E70" t="s">
+        <v>18</v>
+      </c>
+      <c r="F70" s="2">
+        <v>44698</v>
+      </c>
+      <c r="G70">
+        <v>0.0026</v>
+      </c>
+      <c r="H70">
+        <v>15.46</v>
+      </c>
+      <c r="I70" t="s">
+        <v>19</v>
+      </c>
+      <c r="J70" t="s">
+        <v>64</v>
+      </c>
+      <c r="K70" t="s">
+        <v>137</v>
+      </c>
+      <c r="L70">
+        <v>-2000</v>
+      </c>
+      <c r="M70">
+        <v>-2000</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13">
+      <c r="A71" s="1">
+        <v>81</v>
+      </c>
+      <c r="B71" s="2">
+        <v>44657</v>
+      </c>
+      <c r="C71" t="s">
+        <v>12</v>
+      </c>
+      <c r="D71" t="s">
+        <v>13</v>
+      </c>
+      <c r="E71" t="s">
+        <v>18</v>
+      </c>
+      <c r="F71" s="2">
+        <v>44699</v>
+      </c>
+      <c r="G71">
+        <v>0.0026</v>
+      </c>
+      <c r="H71">
+        <v>15.41</v>
+      </c>
+      <c r="I71" t="s">
+        <v>19</v>
+      </c>
+      <c r="J71" t="s">
+        <v>64</v>
+      </c>
+      <c r="K71" t="s">
+        <v>138</v>
+      </c>
+      <c r="L71">
+        <v>-3184</v>
+      </c>
+      <c r="M71">
+        <v>-300</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13">
+      <c r="A72" s="1">
+        <v>82</v>
+      </c>
+      <c r="B72" s="2">
+        <v>44649</v>
+      </c>
+      <c r="C72" t="s">
+        <v>12</v>
+      </c>
+      <c r="D72" t="s">
+        <v>13</v>
+      </c>
+      <c r="E72" t="s">
+        <v>18</v>
+      </c>
+      <c r="F72" s="2">
+        <v>44691</v>
+      </c>
+      <c r="G72">
+        <v>0.0016</v>
+      </c>
+      <c r="H72">
+        <v>57.28</v>
+      </c>
+      <c r="I72" t="s">
+        <v>19</v>
+      </c>
+      <c r="J72" t="s">
+        <v>65</v>
+      </c>
+      <c r="K72" t="s">
+        <v>139</v>
+      </c>
+      <c r="L72">
+        <v>-1406</v>
+      </c>
+      <c r="M72">
+        <v>-1406</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13">
+      <c r="A73" s="1">
+        <v>83</v>
+      </c>
+      <c r="B73" s="2">
+        <v>44650</v>
+      </c>
+      <c r="C73" t="s">
+        <v>12</v>
+      </c>
+      <c r="D73" t="s">
+        <v>13</v>
+      </c>
+      <c r="E73" t="s">
+        <v>18</v>
+      </c>
+      <c r="F73" s="2">
+        <v>44692</v>
+      </c>
+      <c r="G73">
+        <v>0.0016</v>
+      </c>
+      <c r="H73">
+        <v>57.01</v>
+      </c>
+      <c r="I73" t="s">
+        <v>19</v>
+      </c>
+      <c r="J73" t="s">
+        <v>65</v>
+      </c>
+      <c r="K73" t="s">
+        <v>140</v>
+      </c>
+      <c r="L73">
+        <v>-200</v>
+      </c>
+      <c r="M73">
+        <v>-200</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13">
+      <c r="A74" s="1">
+        <v>84</v>
+      </c>
+      <c r="B74" s="2">
+        <v>44656</v>
+      </c>
+      <c r="C74" t="s">
+        <v>12</v>
+      </c>
+      <c r="D74" t="s">
+        <v>17</v>
+      </c>
+      <c r="E74" t="s">
+        <v>18</v>
+      </c>
+      <c r="F74" s="2">
+        <v>44698</v>
+      </c>
+      <c r="G74">
+        <v>0.008500000000000001</v>
+      </c>
+      <c r="H74">
+        <v>14.44</v>
+      </c>
+      <c r="I74" t="s">
+        <v>19</v>
+      </c>
+      <c r="J74" t="s">
+        <v>66</v>
+      </c>
+      <c r="K74" t="s">
+        <v>141</v>
+      </c>
+      <c r="L74">
+        <v>-3200</v>
+      </c>
+      <c r="M74">
+        <v>-3200</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13">
+      <c r="A75" s="1">
+        <v>85</v>
+      </c>
+      <c r="B75" s="2">
+        <v>44651</v>
+      </c>
+      <c r="C75" t="s">
+        <v>12</v>
+      </c>
+      <c r="D75" t="s">
+        <v>13</v>
+      </c>
+      <c r="E75" t="s">
+        <v>18</v>
+      </c>
+      <c r="F75" s="2">
+        <v>44693</v>
+      </c>
+      <c r="G75">
+        <v>0.008399999999999999</v>
+      </c>
+      <c r="H75">
+        <v>14.59</v>
+      </c>
+      <c r="I75" t="s">
+        <v>19</v>
+      </c>
+      <c r="J75" t="s">
+        <v>66</v>
+      </c>
+      <c r="K75" t="s">
+        <v>142</v>
+      </c>
+      <c r="L75">
+        <v>-900</v>
+      </c>
+      <c r="M75">
+        <v>-900</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13">
+      <c r="A76" s="1">
+        <v>86</v>
+      </c>
+      <c r="B76" s="2">
+        <v>44657</v>
+      </c>
+      <c r="C76" t="s">
+        <v>12</v>
+      </c>
+      <c r="D76" t="s">
+        <v>13</v>
+      </c>
+      <c r="E76" t="s">
+        <v>18</v>
+      </c>
+      <c r="F76" s="2">
+        <v>44699</v>
+      </c>
+      <c r="G76">
+        <v>0.008500000000000001</v>
+      </c>
+      <c r="H76">
+        <v>14.32</v>
+      </c>
+      <c r="I76" t="s">
+        <v>19</v>
+      </c>
+      <c r="J76" t="s">
+        <v>66</v>
+      </c>
+      <c r="K76" t="s">
+        <v>143</v>
+      </c>
+      <c r="L76">
+        <v>-3816</v>
+      </c>
+      <c r="M76">
+        <v>-1100</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13">
+      <c r="A77" s="1">
+        <v>88</v>
+      </c>
+      <c r="B77" s="2">
+        <v>44650</v>
+      </c>
+      <c r="C77" t="s">
+        <v>12</v>
+      </c>
+      <c r="D77" t="s">
+        <v>13</v>
+      </c>
+      <c r="E77" t="s">
+        <v>18</v>
+      </c>
+      <c r="F77" s="2">
+        <v>44692</v>
+      </c>
+      <c r="G77">
+        <v>0.0068</v>
+      </c>
+      <c r="H77">
+        <v>24.48</v>
+      </c>
+      <c r="I77" t="s">
+        <v>19</v>
+      </c>
+      <c r="J77" t="s">
+        <v>67</v>
+      </c>
+      <c r="K77" t="s">
+        <v>144</v>
+      </c>
+      <c r="L77">
+        <v>-3650</v>
+      </c>
+      <c r="M77">
+        <v>-3650</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13">
+      <c r="A78" s="1">
+        <v>89</v>
+      </c>
+      <c r="B78" s="2">
+        <v>44644</v>
+      </c>
+      <c r="C78" t="s">
+        <v>12</v>
+      </c>
+      <c r="D78" t="s">
+        <v>13</v>
+      </c>
+      <c r="E78" t="s">
+        <v>18</v>
+      </c>
+      <c r="F78" s="2">
+        <v>44686</v>
+      </c>
+      <c r="G78">
+        <v>0.0057</v>
+      </c>
+      <c r="H78">
+        <v>23.98</v>
+      </c>
+      <c r="I78" t="s">
+        <v>19</v>
+      </c>
+      <c r="J78" t="s">
+        <v>67</v>
+      </c>
+      <c r="K78" t="s">
+        <v>145</v>
+      </c>
+      <c r="L78">
+        <v>-8779</v>
+      </c>
+      <c r="M78">
+        <v>-5550</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13">
+      <c r="A79" s="1">
+        <v>90</v>
+      </c>
+      <c r="B79" s="2">
+        <v>44650</v>
+      </c>
+      <c r="C79" t="s">
+        <v>12</v>
+      </c>
+      <c r="D79" t="s">
+        <v>13</v>
+      </c>
+      <c r="E79" t="s">
+        <v>18</v>
+      </c>
+      <c r="F79" s="2">
+        <v>44692</v>
+      </c>
+      <c r="G79">
+        <v>0.0231</v>
+      </c>
+      <c r="H79">
+        <v>21.4</v>
+      </c>
+      <c r="I79" t="s">
+        <v>19</v>
+      </c>
+      <c r="J79" t="s">
+        <v>68</v>
+      </c>
+      <c r="K79" t="s">
+        <v>146</v>
+      </c>
+      <c r="L79">
+        <v>-3106</v>
+      </c>
+      <c r="M79">
+        <v>-1300</v>
       </c>
     </row>
   </sheetData>

</xml_diff>